<commit_message>
added graphs to check normal assumtions
</commit_message>
<xml_diff>
--- a/dataframeResult.xlsx
+++ b/dataframeResult.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>x1</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>mu</t>
+  </si>
+  <si>
+    <t>dev</t>
   </si>
 </sst>
 </file>
@@ -389,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +417,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>8135</v>
       </c>
@@ -434,8 +440,11 @@
       <c r="F2">
         <v>97.7314131427339</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>-5.603313142733896</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1629</v>
       </c>
@@ -454,8 +463,11 @@
       <c r="F3">
         <v>38.93081868667689</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>13.44178131332311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2824</v>
       </c>
@@ -474,8 +486,11 @@
       <c r="F4">
         <v>49.73111231947556</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>-0.4109123194755568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>9780</v>
       </c>
@@ -494,8 +509,11 @@
       <c r="F5">
         <v>201.6683178554934</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>-5.847117855493366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>8856</v>
       </c>
@@ -514,8 +532,11 @@
       <c r="F6">
         <v>104.2477409328994</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>-3.445840932899443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>10387</v>
       </c>
@@ -534,8 +555,11 @@
       <c r="F7">
         <v>118.084769846552</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>-4.373669846551962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>4002</v>
       </c>
@@ -554,8 +578,11 @@
       <c r="F8">
         <v>60.37776160770719</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>-5.789761607707192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>9572</v>
       </c>
@@ -574,8 +601,11 @@
       <c r="F9">
         <v>197.8941122881936</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>18.23958771180645</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9177</v>
       </c>
@@ -594,8 +624,11 @@
       <c r="F10">
         <v>107.1489076744295</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>15.18559232557055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9304</v>
       </c>
@@ -614,8 +647,11 @@
       <c r="F11">
         <v>193.0311935764804</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>5.145006423519618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>5354</v>
       </c>
@@ -634,8 +670,11 @@
       <c r="F12">
         <v>72.59700595209532</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>-1.529305952095314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>6405</v>
       </c>
@@ -654,8 +693,11 @@
       <c r="F13">
         <v>140.4282034822395</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>-10.90580348223946</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>10135</v>
       </c>
@@ -674,8 +716,11 @@
       <c r="F14">
         <v>115.8072183859116</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>5.692681614088414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>6977</v>
       </c>
@@ -694,8 +739,11 @@
       <c r="F15">
         <v>150.8072687923139</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>-6.725968792313893</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1068</v>
       </c>
@@ -714,8 +762,11 @@
       <c r="F16">
         <v>33.86055531596554</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>-1.741455315965538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>3723</v>
       </c>
@@ -734,8 +785,11 @@
       <c r="F17">
         <v>91.76272592696031</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>1.749274073039686</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>2374</v>
       </c>
@@ -754,8 +808,11 @@
       <c r="F18">
         <v>67.28482539673232</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>-3.701725396732314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>8086</v>
       </c>
@@ -774,8 +831,11 @@
       <c r="F19">
         <v>97.28855591427605</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>0.3376440857239515</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1415</v>
       </c>
@@ -794,8 +854,11 @@
       <c r="F20">
         <v>49.88356030519142</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>-2.300460305191415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>5367</v>
       </c>
@@ -814,8 +877,11 @@
       <c r="F21">
         <v>72.71449868617597</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>17.32180131382403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>7803</v>
       </c>
@@ -834,8 +900,11 @@
       <c r="F22">
         <v>165.7952197470717</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>17.56528025292826</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>6517</v>
       </c>
@@ -854,8 +923,11 @@
       <c r="F23">
         <v>83.10808670100315</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>17.30731329899686</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>2779</v>
       </c>
@@ -874,8 +946,11 @@
       <c r="F24">
         <v>49.32440670150405</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>5.523193298495954</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>1855</v>
       </c>
@@ -894,8 +969,11 @@
       <c r="F25">
         <v>57.86745669755637</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>-1.493256697556369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2867</v>
       </c>
@@ -914,8 +992,11 @@
       <c r="F26">
         <v>50.11974213220387</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>-2.348742132203867</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>4687</v>
       </c>
@@ -934,8 +1015,11 @@
       <c r="F27">
         <v>66.56872490349558</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>-2.357624903495577</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>10310</v>
       </c>
@@ -954,8 +1038,11 @@
       <c r="F28">
         <v>117.3888513446896</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>4.589348655310374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>7966</v>
       </c>
@@ -974,8 +1061,11 @@
       <c r="F29">
         <v>96.20400759968538</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>-7.611607599685385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>2663</v>
       </c>
@@ -994,8 +1084,11 @@
       <c r="F30">
         <v>48.27600999739975</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>-1.096309997399757</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>8735</v>
       </c>
@@ -1014,8 +1107,11 @@
       <c r="F31">
         <v>103.1541547156872</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>-12.54295471568719</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>5132</v>
       </c>
@@ -1034,8 +1130,11 @@
       <c r="F32">
         <v>70.59059157010259</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>5.806808429897416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>8086</v>
       </c>
@@ -1054,8 +1153,11 @@
       <c r="F33">
         <v>170.9303167448883</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>-2.229316744888308</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>4321</v>
       </c>
@@ -1074,8 +1176,11 @@
       <c r="F34">
         <v>102.6135669329472</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>-13.79736693294724</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>6510</v>
       </c>
@@ -1094,8 +1199,11 @@
       <c r="F35">
         <v>83.044821382652</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>-7.247221382652</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>10964</v>
       </c>
@@ -1114,8 +1222,11 @@
       <c r="F36">
         <v>223.1522572385846</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>-0.1143572385845459</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>7671</v>
       </c>
@@ -1134,8 +1245,11 @@
       <c r="F37">
         <v>163.4000508293622</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>-6.271950829362254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>9889</v>
       </c>
@@ -1154,8 +1268,11 @@
       <c r="F38">
         <v>203.646146734511</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>-1.583546734511032</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>4582</v>
       </c>
@@ -1174,8 +1291,11 @@
       <c r="F39">
         <v>107.3494691111455</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>6.069930888854458</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>5340</v>
       </c>
@@ -1194,8 +1314,11 @@
       <c r="F40">
         <v>121.1035451689015</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>-0.3655451689015479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>8330</v>
       </c>
@@ -1214,8 +1337,11 @@
       <c r="F41">
         <v>99.49380415394371</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>-20.29510415394371</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>10945</v>
       </c>
@@ -1234,8 +1360,11 @@
       <c r="F42">
         <v>123.1279195093985</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>9.86518049060146</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>5766</v>
       </c>
@@ -1254,8 +1383,11 @@
       <c r="F43">
         <v>76.32062183218991</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>-2.231821832189908</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>4315</v>
       </c>
@@ -1274,8 +1406,11 @@
       <c r="F44">
         <v>63.20662512826451</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>3.278374871735487</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>7053</v>
       </c>
@@ -1294,8 +1429,11 @@
       <c r="F45">
         <v>152.1863054419042</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>-9.537505441904216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>8731</v>
       </c>
@@ -1314,8 +1452,11 @@
       <c r="F46">
         <v>103.1180031052008</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>-6.112103105200845</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>4856</v>
       </c>
@@ -1334,8 +1475,11 @@
       <c r="F47">
         <v>68.09613044654407</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>7.117969553455936</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>3038</v>
       </c>
@@ -1354,8 +1498,11 @@
       <c r="F48">
         <v>51.66522348049555</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>-15.57292348049555</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>4866</v>
       </c>
@@ -1374,8 +1521,11 @@
       <c r="F49">
         <v>112.5027113280356</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>4.23158867196436</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>1650</v>
       </c>
@@ -1394,8 +1544,11 @@
       <c r="F50">
         <v>54.14768678747724</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>13.48211321252276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>5323</v>
       </c>
@@ -1413,6 +1566,9 @@
       </c>
       <c r="F51">
         <v>120.7950764446511</v>
+      </c>
+      <c r="G51">
+        <v>-6.76587644465107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>